<commit_message>
Updates to ODH IG
</commit_message>
<xml_diff>
--- a/docs/odh/odh-Employer-extension.xlsx
+++ b/docs/odh/odh-Employer-extension.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="70">
   <si>
     <t>Path</t>
   </si>
@@ -138,30 +138,30 @@
   </si>
   <si>
     <t>A person or organization that hires the services of another.</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1
 </t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {children().count() &gt; id.count()}
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>Extension.id</t>
   </si>
   <si>
-    <t xml:space="preserve">string {[]} {[]}
+    <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string
 </t>
   </si>
   <si>
-    <t>xml:id (or equivalent in JSON)</t>
-  </si>
-  <si>
-    <t>unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
   </si>
   <si>
     <t>Element.id</t>
@@ -170,11 +170,31 @@
     <t>Extension.extension</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[]} {[]}
+    <t>extensions
+user content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension
 </t>
   </si>
   <si>
-    <t>An Extension</t>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
   </si>
   <si>
     <t>Element.extension</t>
@@ -183,7 +203,7 @@
     <t>Extension.url</t>
   </si>
   <si>
-    <t xml:space="preserve">uri {[]} {[]}
+    <t xml:space="preserve">uri
 </t>
   </si>
   <si>
@@ -193,20 +213,26 @@
     <t>Source of the definition for the extension code - a logical name or a URL.</t>
   </si>
   <si>
-    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://hl7.org/fhir/us/odh/StructureDefinition/odh-Employer-extension"/&gt;</t>
+    <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/odh/StructureDefinition/odh-Employer-extension</t>
+  </si>
+  <si>
+    <t>Extension.valueReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/odh/StructureDefinition/odh-EmployerPerson|http://hl7.org/fhir/us/odh/StructureDefinition/obf-Organization)
+</t>
+  </si>
+  <si>
+    <t>Value of extension</t>
+  </si>
+  <si>
+    <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](extensibility.html) for a list).</t>
   </si>
   <si>
     <t>Extension.value[x]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/odh/StructureDefinition/odh-EmployerPerson], CanonicalType[http://hl7.org/fhir/us/odh/StructureDefinition/shr-core-Organization]]}
-</t>
-  </si>
-  <si>
-    <t>Value of extension</t>
-  </si>
-  <si>
-    <t>Value of extension - may be a resource or one of a constrained set of the data types (see Extensibility in the spec for list).</t>
   </si>
 </sst>
 </file>
@@ -259,67 +285,67 @@
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin"/>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin"/>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin"/>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
   </borders>
@@ -364,9 +390,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.00390625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="24.1875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="12.3828125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
@@ -374,7 +400,7 @@
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="36.0859375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="43.421875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -391,7 +417,7 @@
     <col min="25" max="25" width="17.07421875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="17.7265625" customWidth="true" bestFit="true" hidden="true"/>
@@ -596,18 +622,18 @@
         <v>37</v>
       </c>
       <c r="AG2" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH2" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AH2" t="s" s="2">
+      <c r="AI2" t="s" s="2">
         <v>42</v>
-      </c>
-      <c r="AI2" t="s" s="2">
-        <v>43</v>
       </c>
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -618,7 +644,7 @@
         <v>37</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s" s="2">
         <v>36</v>
@@ -693,7 +719,7 @@
         <v>37</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AH3" t="s" s="2">
         <v>36</v>
@@ -708,7 +734,7 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
@@ -727,15 +753,17 @@
         <v>36</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="M4" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="M4" t="s" s="2">
+        <v>54</v>
+      </c>
       <c r="N4" s="2"/>
       <c r="O4" t="s" s="2">
         <v>36</v>
@@ -772,19 +800,19 @@
         <v>36</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="AC4" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>37</v>
@@ -801,7 +829,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -809,10 +837,10 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s" s="2">
         <v>36</v>
@@ -824,22 +852,24 @@
         <v>36</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="M5" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="M5" t="s" s="2">
+        <v>63</v>
+      </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
         <v>36</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" t="s" s="2">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="R5" t="s" s="2">
         <v>36</v>
@@ -881,13 +911,13 @@
         <v>36</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AH5" t="s" s="2">
         <v>36</v>
@@ -898,7 +928,7 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -906,10 +936,10 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s" s="2">
         <v>36</v>
@@ -921,13 +951,13 @@
         <v>36</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -978,13 +1008,13 @@
         <v>36</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AH6" t="s" s="2">
         <v>36</v>

</xml_diff>